<commit_message>
Update Properties and Methods Spreadsheet
</commit_message>
<xml_diff>
--- a/Software/OpenAstroTracker ASCOM/ASCOM Methods and Properties.xlsx
+++ b/Software/OpenAstroTracker ASCOM/ASCOM Methods and Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Git\OpenAstroTracker\Software\OpenAstroTracker ASCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF4EF4B2-97D2-488E-89E1-8DAA141A7CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBB793A-7A3B-415A-978E-AB9FBC3B32CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="9450" windowWidth="29040" windowHeight="15840" xr2:uid="{726BEF06-5338-4E9A-B5F9-49858C6239A8}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{726BEF06-5338-4E9A-B5F9-49858C6239A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ASCOM ItelescopeV3 Methods" sheetId="1" r:id="rId1"/>
@@ -977,7 +977,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,13 +1173,13 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E809B9-9EA3-43A2-B5B8-1E4861539A25}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1527,7 @@
         <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1897,13 +1897,13 @@
         <v>121</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>122</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ASCOM 0.3.0.0 - Updates
- Added Slew rate support to MoveAxis
</commit_message>
<xml_diff>
--- a/Software/OpenAstroTracker ASCOM/ASCOM Methods and Properties.xlsx
+++ b/Software/OpenAstroTracker ASCOM/ASCOM Methods and Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Git\OpenAstroTracker\Software\OpenAstroTracker ASCOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lutz.KRETZSCHMAR.000\Source\OpenAstroTracker\Software\OpenAstroTracker ASCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBB793A-7A3B-415A-978E-AB9FBC3B32CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7707C09F-95C7-42D0-AD2C-F3FC9CED8F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{726BEF06-5338-4E9A-B5F9-49858C6239A8}"/>
+    <workbookView xWindow="6270" yWindow="2925" windowWidth="28800" windowHeight="17235" xr2:uid="{726BEF06-5338-4E9A-B5F9-49858C6239A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ASCOM ItelescopeV3 Methods" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>UTC Date</t>
+  </si>
+  <si>
+    <t>0.3.0.0</t>
+  </si>
+  <si>
+    <t>0.2.0.0</t>
   </si>
 </sst>
 </file>
@@ -974,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21215E10-4F9F-40B7-BD0B-29A9E03E8C81}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +995,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1013,8 +1019,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1027,8 +1036,11 @@
       <c r="D3" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1041,8 +1053,11 @@
       <c r="D4" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1055,8 +1070,11 @@
       <c r="D5" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1069,8 +1087,11 @@
       <c r="D6" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1083,8 +1104,11 @@
       <c r="D7" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1097,8 +1121,11 @@
       <c r="D8" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1139,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1125,8 +1152,11 @@
       <c r="D10" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1140,12 +1170,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
@@ -1153,8 +1183,11 @@
       <c r="D12" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1167,8 +1200,11 @@
       <c r="D13" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1181,8 +1217,11 @@
       <c r="D14" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1235,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1209,8 +1248,11 @@
       <c r="D16" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1224,7 +1266,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1238,7 +1280,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1251,8 +1293,11 @@
       <c r="D19" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1265,8 +1310,11 @@
       <c r="D20" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1279,8 +1327,11 @@
       <c r="D21" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1293,8 +1344,11 @@
       <c r="D22" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1308,7 +1362,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1321,8 +1375,11 @@
       <c r="D24" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1335,8 +1392,11 @@
       <c r="D25" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1348,6 +1408,9 @@
       </c>
       <c r="D26" s="1" t="s">
         <v>170</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>